<commit_message>
Dictionnaire de données fini
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -5,16 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\59011-14-01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Partage\projet_hotel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28065" windowHeight="10470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dictionnaire de données" sheetId="1" r:id="rId1"/>
+    <sheet name="Organisé par entité" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,20 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="129">
   <si>
     <t>Nom</t>
   </si>
   <si>
-    <t>Libellé</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>IdEmploye</t>
   </si>
   <si>
@@ -197,33 +193,9 @@
     <t>DECIMAL</t>
   </si>
   <si>
-    <t>IdReservation</t>
-  </si>
-  <si>
-    <t>Identifiant de la réservation</t>
-  </si>
-  <si>
-    <t>NumReservation</t>
-  </si>
-  <si>
-    <t>Numéro de la réservation</t>
-  </si>
-  <si>
-    <t>DateDebutReservation</t>
-  </si>
-  <si>
-    <t>Date de début de la réservation</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>DateFinReservation</t>
-  </si>
-  <si>
-    <t>Date de fin de la réservation</t>
-  </si>
-  <si>
     <t>NbPersonnes</t>
   </si>
   <si>
@@ -284,21 +256,6 @@
     <t>Pourcentage de réduction appliqué au type de client</t>
   </si>
   <si>
-    <t>HistoriquePrixPrestation</t>
-  </si>
-  <si>
-    <t>HistoriquePrixChambre</t>
-  </si>
-  <si>
-    <t>HistoriqueReservation</t>
-  </si>
-  <si>
-    <t>HistoriqueFacturation</t>
-  </si>
-  <si>
-    <t>HistoriqueNettoyage</t>
-  </si>
-  <si>
     <t>IdNettoyage</t>
   </si>
   <si>
@@ -327,13 +284,142 @@
   </si>
   <si>
     <t>Libellé du type d'employé</t>
+  </si>
+  <si>
+    <t>Définition</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>DateDebutPrixPrestation</t>
+  </si>
+  <si>
+    <t>Date de début d'application du prix de la prestation</t>
+  </si>
+  <si>
+    <t>DateDebutPrixChambre</t>
+  </si>
+  <si>
+    <t>Date de début d'application du prix de la chambre</t>
+  </si>
+  <si>
+    <t>IdFacture</t>
+  </si>
+  <si>
+    <t>Identifiant de la facture</t>
+  </si>
+  <si>
+    <t>NumFacture</t>
+  </si>
+  <si>
+    <t>Numéro de la facture</t>
+  </si>
+  <si>
+    <t>IdReservationSejour</t>
+  </si>
+  <si>
+    <t>Identifiant de la réservation du séjour</t>
+  </si>
+  <si>
+    <t>NumReservationSejour</t>
+  </si>
+  <si>
+    <t>Numéro de la réservation du séjour</t>
+  </si>
+  <si>
+    <t>DateDebutReservationSejour</t>
+  </si>
+  <si>
+    <t>Date de début de la réservation du séjour</t>
+  </si>
+  <si>
+    <t>DateFinReservationSejour</t>
+  </si>
+  <si>
+    <t>Date de fin de la réservation du séjour</t>
+  </si>
+  <si>
+    <t>IdReservationPrestation</t>
+  </si>
+  <si>
+    <t>Identifiant de la réservation de la prestation</t>
+  </si>
+  <si>
+    <t>DateReservationPrestation</t>
+  </si>
+  <si>
+    <t>Date et heure de la prestation réservée</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>QuantitePrestation</t>
+  </si>
+  <si>
+    <t>Quantité de la prestation réservée</t>
+  </si>
+  <si>
+    <t>DateFacture</t>
+  </si>
+  <si>
+    <t>Date d'émission de la facture</t>
+  </si>
+  <si>
+    <t>DateHeureNettoyage</t>
+  </si>
+  <si>
+    <t>Date et heure à laquelle le nettoyage a été réalisé</t>
+  </si>
+  <si>
+    <t>TypesChambres</t>
+  </si>
+  <si>
+    <t>EquipementsChambres</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>Employés</t>
+  </si>
+  <si>
+    <t>Chambres</t>
+  </si>
+  <si>
+    <t>Prestations</t>
+  </si>
+  <si>
+    <t>ReservationsSejours</t>
+  </si>
+  <si>
+    <t>Fidelites</t>
+  </si>
+  <si>
+    <t>StatutChambres</t>
+  </si>
+  <si>
+    <t>TypesClients</t>
+  </si>
+  <si>
+    <t>Nettoyages</t>
+  </si>
+  <si>
+    <t>TypesEmployes</t>
+  </si>
+  <si>
+    <t>Factures</t>
+  </si>
+  <si>
+    <t>ReservationsPrestations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,13 +427,104 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF996633"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -473,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -501,31 +678,183 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -617,38 +946,204 @@
     <dxf>
       <border>
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF996633"/>
+      <color rgb="FF66FFFF"/>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -661,13 +1156,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D51" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:D51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D62" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:D62"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Nom" dataDxfId="4"/>
-    <tableColumn id="2" name="Libellé" dataDxfId="3"/>
-    <tableColumn id="3" name="Type" dataDxfId="2"/>
-    <tableColumn id="4" name="Code" dataDxfId="1"/>
+    <tableColumn id="1" name="Nom" dataDxfId="12"/>
+    <tableColumn id="2" name="Définition" dataDxfId="11"/>
+    <tableColumn id="3" name="Type" dataDxfId="10"/>
+    <tableColumn id="4" name="Notes" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:D60" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D60"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Nom" dataDxfId="3"/>
+    <tableColumn id="2" name="Définition" dataDxfId="2"/>
+    <tableColumn id="3" name="Type" dataDxfId="1"/>
+    <tableColumn id="4" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -937,15 +1445,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
@@ -955,584 +1463,694 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
+        <v>76</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="9"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="6"/>
+      <c r="C46" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D48" s="6"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
+      <c r="A51" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1540,4 +2158,753 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="G2" s="65" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="G3" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="G4" s="66" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="G5" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="G6" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="G7" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="G8" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="G9" s="36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="G10" s="44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="G11" s="46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="G12" s="54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="G13" s="56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="G14" s="61" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="G15" s="63" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="31"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="28"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="34"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="34"/>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="34"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="34"/>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="34"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="34"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="37"/>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="37"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="40"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="43"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="47"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="47"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="47"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="50"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="53"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="53"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="57"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="57"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="60"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="60"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="60"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="64"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="64"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="64"/>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="9"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MCD sans relations + MAJ Dictionnaire de données
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Organisé par entité" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="135">
   <si>
     <t>Nom</t>
   </si>
@@ -413,6 +412,24 @@
   </si>
   <si>
     <t>ReservationsPrestations</t>
+  </si>
+  <si>
+    <t>IdEtage</t>
+  </si>
+  <si>
+    <t>NumEtage</t>
+  </si>
+  <si>
+    <t>Identifiant de l'étage</t>
+  </si>
+  <si>
+    <t>Numéro de l'étage</t>
+  </si>
+  <si>
+    <t>Etages</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -435,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,8 +543,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -646,11 +669,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -849,6 +887,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,7 +1498,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="A54" sqref="A54:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,7 +1678,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
@@ -2099,15 +2149,27 @@
       <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="A54" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
+      <c r="A55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2447,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>30</v>
       </c>
@@ -2411,8 +2473,11 @@
         <v>8</v>
       </c>
       <c r="D16" s="25"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16" s="70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>35</v>
       </c>
@@ -2424,7 +2489,7 @@
       </c>
       <c r="D17" s="25"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>44</v>
       </c>
@@ -2436,7 +2501,7 @@
       </c>
       <c r="D18" s="25"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
@@ -2448,7 +2513,7 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>39</v>
       </c>
@@ -2462,7 +2527,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>42</v>
       </c>
@@ -2474,7 +2539,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>46</v>
       </c>
@@ -2486,7 +2551,7 @@
       </c>
       <c r="D22" s="28"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>48</v>
       </c>
@@ -2498,7 +2563,7 @@
       </c>
       <c r="D23" s="28"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>50</v>
       </c>
@@ -2510,7 +2575,7 @@
       </c>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>52</v>
       </c>
@@ -2522,7 +2587,7 @@
       </c>
       <c r="D25" s="28"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>96</v>
       </c>
@@ -2534,7 +2599,7 @@
       </c>
       <c r="D26" s="34"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>98</v>
       </c>
@@ -2546,7 +2611,7 @@
       </c>
       <c r="D27" s="34"/>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
         <v>100</v>
       </c>
@@ -2558,7 +2623,7 @@
       </c>
       <c r="D28" s="34"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>102</v>
       </c>
@@ -2570,7 +2635,7 @@
       </c>
       <c r="D29" s="34"/>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>56</v>
       </c>
@@ -2581,8 +2646,11 @@
         <v>8</v>
       </c>
       <c r="D30" s="34"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>58</v>
       </c>
@@ -2593,8 +2661,11 @@
         <v>8</v>
       </c>
       <c r="D31" s="34"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
         <v>60</v>
       </c>
@@ -2822,53 +2893,65 @@
       </c>
       <c r="D50" s="64"/>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="69"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="69"/>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B53" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="6"/>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B54" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="6"/>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B55" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="9"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>

</xml_diff>

<commit_message>
MCD avec relations, version non définitive
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="140">
   <si>
     <t>Nom</t>
   </si>
@@ -430,6 +430,21 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>IdTypePaiement</t>
+  </si>
+  <si>
+    <t>Identifiant du type de paiement</t>
+  </si>
+  <si>
+    <t>LibelleTypePaiement</t>
+  </si>
+  <si>
+    <t>Libelle du type de paiement</t>
+  </si>
+  <si>
+    <t>Libellé du type de paiement</t>
   </si>
 </sst>
 </file>
@@ -452,7 +467,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +561,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -898,6 +919,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -998,13 +1028,6 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1025,6 +1048,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1219,8 +1249,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:D60" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:D62" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D62"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Nom" dataDxfId="3"/>
     <tableColumn id="2" name="Définition" dataDxfId="2"/>
@@ -1497,8 +1527,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:D55"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,15 +2203,27 @@
       <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
+      <c r="A56" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
+      <c r="A57" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,10 +2266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2917,53 +2959,65 @@
       </c>
       <c r="D52" s="69"/>
     </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="73"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="73"/>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B55" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B57" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
@@ -2978,10 +3032,22 @@
       <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="9"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dictionnaire de données V2 + agencement MCD
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="126">
   <si>
     <t>Nom</t>
   </si>
@@ -87,12 +87,6 @@
     <t>Prénom du client</t>
   </si>
   <si>
-    <t>NumClient</t>
-  </si>
-  <si>
-    <t>Numéro de client</t>
-  </si>
-  <si>
     <t>MailClient</t>
   </si>
   <si>
@@ -153,12 +147,6 @@
     <t>1er numéro = étage</t>
   </si>
   <si>
-    <t>EtageChambre</t>
-  </si>
-  <si>
-    <t>Étage de la Chambre</t>
-  </si>
-  <si>
     <t>PrixChambre</t>
   </si>
   <si>
@@ -237,42 +225,9 @@
     <t>Libellé du statut de la chambre</t>
   </si>
   <si>
-    <t>IdTypeClient</t>
-  </si>
-  <si>
-    <t>Identifiant du type de client</t>
-  </si>
-  <si>
-    <t>LibelleTypeClient</t>
-  </si>
-  <si>
-    <t>Libellé du type de client</t>
-  </si>
-  <si>
     <t>PourcentageReduction</t>
   </si>
   <si>
-    <t>Pourcentage de réduction appliqué au type de client</t>
-  </si>
-  <si>
-    <t>IdNettoyage</t>
-  </si>
-  <si>
-    <t>Identifiant du nettoyage</t>
-  </si>
-  <si>
-    <t>LibelleNettoyage</t>
-  </si>
-  <si>
-    <t>Libellé du nettoyage</t>
-  </si>
-  <si>
-    <t>DescriptionNettoyage</t>
-  </si>
-  <si>
-    <t>Description du nettoyage</t>
-  </si>
-  <si>
     <t>IdTypeEmploye</t>
   </si>
   <si>
@@ -291,24 +246,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>DateDebutPrixPrestation</t>
-  </si>
-  <si>
-    <t>Date de début d'application du prix de la prestation</t>
-  </si>
-  <si>
-    <t>DateDebutPrixChambre</t>
-  </si>
-  <si>
-    <t>Date de début d'application du prix de la chambre</t>
-  </si>
-  <si>
-    <t>IdFacture</t>
-  </si>
-  <si>
-    <t>Identifiant de la facture</t>
-  </si>
-  <si>
     <t>NumFacture</t>
   </si>
   <si>
@@ -339,33 +276,12 @@
     <t>Date de fin de la réservation du séjour</t>
   </si>
   <si>
-    <t>IdReservationPrestation</t>
-  </si>
-  <si>
-    <t>Identifiant de la réservation de la prestation</t>
-  </si>
-  <si>
-    <t>DateReservationPrestation</t>
-  </si>
-  <si>
-    <t>Date et heure de la prestation réservée</t>
-  </si>
-  <si>
     <t>DATETIME</t>
   </si>
   <si>
     <t>QuantitePrestation</t>
   </si>
   <si>
-    <t>Quantité de la prestation réservée</t>
-  </si>
-  <si>
-    <t>DateFacture</t>
-  </si>
-  <si>
-    <t>Date d'émission de la facture</t>
-  </si>
-  <si>
     <t>DateHeureNettoyage</t>
   </si>
   <si>
@@ -399,21 +315,9 @@
     <t>StatutChambres</t>
   </si>
   <si>
-    <t>TypesClients</t>
-  </si>
-  <si>
-    <t>Nettoyages</t>
-  </si>
-  <si>
     <t>TypesEmployes</t>
   </si>
   <si>
-    <t>Factures</t>
-  </si>
-  <si>
-    <t>ReservationsPrestations</t>
-  </si>
-  <si>
     <t>IdEtage</t>
   </si>
   <si>
@@ -429,9 +333,6 @@
     <t>Etages</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>IdTypePaiement</t>
   </si>
   <si>
@@ -444,7 +345,64 @@
     <t>Libelle du type de paiement</t>
   </si>
   <si>
-    <t>Libellé du type de paiement</t>
+    <t>Siret</t>
+  </si>
+  <si>
+    <t>Numéro de SIRET de l'entreprise</t>
+  </si>
+  <si>
+    <t>NomEntreprise</t>
+  </si>
+  <si>
+    <t>Nom de l'entreprise</t>
+  </si>
+  <si>
+    <t>NumEntreprise</t>
+  </si>
+  <si>
+    <t>Numéro client de l'entreprise</t>
+  </si>
+  <si>
+    <t>Pourcentage de réduction appliqué à l'entreprise</t>
+  </si>
+  <si>
+    <t>NumParticulier</t>
+  </si>
+  <si>
+    <t>Numéro d'un client particulier</t>
+  </si>
+  <si>
+    <t>DateHeureAction</t>
+  </si>
+  <si>
+    <t>Date et heure de l'enregistrement d'une action sur une réservation de séjour</t>
+  </si>
+  <si>
+    <t>DatePrestation</t>
+  </si>
+  <si>
+    <t>Date et heure de la prestation</t>
+  </si>
+  <si>
+    <t>Quantité de la prestation</t>
+  </si>
+  <si>
+    <t>Particuliers</t>
+  </si>
+  <si>
+    <t>TypesPaiements</t>
+  </si>
+  <si>
+    <t>Facturations</t>
+  </si>
+  <si>
+    <t>Entreprises</t>
+  </si>
+  <si>
+    <t>HistoriqueActions</t>
+  </si>
+  <si>
+    <t>HistoriquesNettoyages</t>
   </si>
 </sst>
 </file>
@@ -467,7 +425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,18 +488,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF66CC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -567,6 +513,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -822,24 +792,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -852,15 +804,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -880,27 +823,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -909,16 +831,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -928,6 +877,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1219,9 +1198,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF996633"/>
+      <color rgb="FF33CCCC"/>
+      <color rgb="FFCC0066"/>
       <color rgb="FF66FFFF"/>
       <color rgb="FFFF66CC"/>
+      <color rgb="FF996633"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1236,8 +1217,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D62" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:D62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D52" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:D52"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Nom" dataDxfId="12"/>
     <tableColumn id="2" name="Définition" dataDxfId="11"/>
@@ -1249,8 +1230,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:D62" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:D58" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D58"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Nom" dataDxfId="3"/>
     <tableColumn id="2" name="Définition" dataDxfId="2"/>
@@ -1525,10 +1506,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,13 +1524,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1672,7 +1653,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -1680,11 +1661,11 @@
         <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1692,7 +1673,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="6"/>
     </row>
@@ -1704,19 +1685,19 @@
         <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D15" s="6"/>
     </row>
@@ -1728,31 +1709,31 @@
         <v>34</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="D18" s="6"/>
     </row>
@@ -1766,45 +1747,45 @@
       <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="6"/>
+      <c r="C22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -1814,88 +1795,88 @@
         <v>49</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="9"/>
+      <c r="A24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>8</v>
@@ -1904,41 +1885,41 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C31" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>64</v>
       </c>
@@ -1946,40 +1927,40 @@
         <v>65</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="B36" s="5" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>8</v>
@@ -1988,70 +1969,70 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="9"/>
+      <c r="A40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>8</v>
@@ -2060,58 +2041,58 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>90</v>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>7</v>
@@ -2120,141 +2101,39 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="C49" s="5" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
       <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="6"/>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2266,10 +2145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,13 +2164,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2305,8 +2184,8 @@
         <v>8</v>
       </c>
       <c r="D2" s="19"/>
-      <c r="G2" s="65" t="s">
-        <v>118</v>
+      <c r="G2" s="49" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2321,7 +2200,7 @@
       </c>
       <c r="D3" s="19"/>
       <c r="G3" s="21" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2335,8 +2214,8 @@
         <v>7</v>
       </c>
       <c r="D4" s="19"/>
-      <c r="G4" s="66" t="s">
-        <v>116</v>
+      <c r="G4" s="50" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2351,7 +2230,7 @@
       </c>
       <c r="D5" s="19"/>
       <c r="G5" s="24" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2366,7 +2245,7 @@
       </c>
       <c r="D6" s="19"/>
       <c r="G6" s="13" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2381,7 +2260,7 @@
       </c>
       <c r="D7" s="22"/>
       <c r="G7" s="27" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2396,7 +2275,7 @@
       </c>
       <c r="D8" s="22"/>
       <c r="G8" s="33" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2411,7 +2290,7 @@
       </c>
       <c r="D9" s="22"/>
       <c r="G9" s="36" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2425,8 +2304,8 @@
         <v>7</v>
       </c>
       <c r="D10" s="22"/>
-      <c r="G10" s="44" t="s">
-        <v>123</v>
+      <c r="G10" s="38" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2440,26 +2319,26 @@
         <v>7</v>
       </c>
       <c r="D11" s="22"/>
-      <c r="G11" s="46" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="G11" s="67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="G12" s="54" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="G12" s="68" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>26</v>
       </c>
@@ -2467,11 +2346,11 @@
         <v>27</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="16"/>
-      <c r="G13" s="56" t="s">
-        <v>126</v>
+      <c r="G13" s="40" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2482,26 +2361,26 @@
         <v>29</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D14" s="16"/>
-      <c r="G14" s="61" t="s">
-        <v>127</v>
+      <c r="G14" s="45" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="B15" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="G15" s="63" t="s">
-        <v>128</v>
+      <c r="C15" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="G15" s="47" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2512,38 +2391,44 @@
         <v>34</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="25"/>
-      <c r="G16" s="70" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="G17" s="72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="25"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="G18" s="76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
@@ -2553,47 +2438,47 @@
       <c r="C19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="D19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B20" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="C20" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="28"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="31"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>48</v>
       </c>
@@ -2601,250 +2486,244 @@
         <v>49</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D23" s="28"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="30" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="34"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="34"/>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="31"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="D26" s="34"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="34"/>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B28" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C28" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="34"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="28"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="34"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="34"/>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="33" t="s">
+      <c r="B29" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="34"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>103</v>
-      </c>
       <c r="C29" s="33" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D29" s="34"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="37"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="34"/>
-      <c r="E30" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="B31" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="34"/>
-      <c r="E31" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="37"/>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="37"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="37"/>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="C33" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="60"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="37"/>
+      <c r="C34" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="63"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="39" t="s">
+      <c r="A35" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="66"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="40"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
+      <c r="B36" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="C36" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="41"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="43"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
+      <c r="B37" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="47"/>
+      <c r="C37" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="41"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="46" t="s">
+      <c r="A38" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="47"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="B38" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="47"/>
+      <c r="C38" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="48"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="48"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="50"/>
+      <c r="A40" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="48"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" s="53"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D42" s="53"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B43" s="56" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C43" s="56" t="s">
         <v>8</v>
@@ -2853,201 +2732,135 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="55" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="B44" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="57"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="44"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="44"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="44"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="44"/>
+    </row>
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="71"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="57"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="60"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="60"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="D47" s="60"/>
-    </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="62" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" s="63" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="64"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="B49" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="C49" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="64"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="64"/>
+      <c r="B50" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="75"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="B51" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="C51" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="69"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="67" t="s">
-        <v>130</v>
-      </c>
-      <c r="B52" s="68" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="69"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="72" t="s">
-        <v>136</v>
-      </c>
-      <c r="C53" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="73"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="B54" s="72" t="s">
-        <v>139</v>
-      </c>
-      <c r="C54" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="73"/>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>55</v>
-      </c>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" s="9"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Maj 12 01 2023 à 08h39
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -2147,15 +2147,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>